<commit_message>
Cleaned up to give email to Skip. All 10 figures now
</commit_message>
<xml_diff>
--- a/PSC-PFTPercentages.xlsx
+++ b/PSC-PFTPercentages.xlsx
@@ -144,10 +144,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -484,19 +485,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -522,7 +524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -551,8 +553,12 @@
         <f>SUM(B2:H2)</f>
         <v>0.9999999879999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="3">
+        <f>C2/B2</f>
+        <v>1.456994220086518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -581,8 +587,12 @@
         <f t="shared" ref="I3:I8" si="0">SUM(B3:H3)</f>
         <v>0.99999994400000014</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J8" si="1">C3/B3</f>
+        <v>1.8720822931678225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -611,8 +621,12 @@
         <f t="shared" si="0"/>
         <v>0.99999999549999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="3">
+        <f t="shared" si="1"/>
+        <v>1.2306768200831213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -621,8 +635,9 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -651,8 +666,12 @@
         <f t="shared" si="0"/>
         <v>1.0000000098999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="3">
+        <f t="shared" si="1"/>
+        <v>1.7845721248171382</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -681,8 +700,12 @@
         <f t="shared" si="0"/>
         <v>1.000000051</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="3">
+        <f t="shared" si="1"/>
+        <v>1.7453857587486827</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -711,8 +734,12 @@
         <f t="shared" si="0"/>
         <v>0.99999998180000005</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J8" s="3">
+        <f t="shared" si="1"/>
+        <v>1.8576789045828714</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>18</v>
       </c>

</xml_diff>